<commit_message>
Capacities min and max now equal, to ensure size is always equal, allow 100% difference for individual timestep flows.
</commit_message>
<xml_diff>
--- a/tests/test_examples/expected_files/results_MPC_example_2018_01_01__00_00_00.xlsx
+++ b/tests/test_examples/expected_files/results_MPC_example_2018_01_01__00_00_00.xlsx
@@ -467,10 +467,10 @@
         <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>3.486082853126365</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.486082853126365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>3.401682853126363</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3.401682853126363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +489,10 @@
         <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>3.389011425126365</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>3.389011425126365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>3.481639996126364</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.481639996126364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -511,10 +511,10 @@
         <v>43101.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>3.558754282126364</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>3.558754282126364</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         <v>43101.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>3.542254282126363</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>3.542254282126363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -533,10 +533,10 @@
         <v>43101.25</v>
       </c>
       <c r="B8" t="n">
-        <v>6.186282853126365</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>6.186282853126365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -544,10 +544,10 @@
         <v>43101.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>5.512620767191083</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>5.512620767191083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -555,10 +555,10 @@
         <v>43101.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>5.890883330042554</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>5.890883330042554</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         <v>43101.375</v>
       </c>
       <c r="B11" t="n">
-        <v>4.232164006801982</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>4.232164006801982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -577,10 +577,10 @@
         <v>43101.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>2.636635328455043</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>2.636635328455043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -588,10 +588,10 @@
         <v>43101.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>4.162432326147626</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>4.162432326147626</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -599,10 +599,10 @@
         <v>43101.5</v>
       </c>
       <c r="B14" t="n">
-        <v>3.384179743762946</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3.384179743762946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -610,10 +610,10 @@
         <v>43101.54166666666</v>
       </c>
       <c r="B15" t="n">
-        <v>1.039761519541608</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.039761519541608</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -621,10 +621,10 @@
         <v>43101.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>2.75835886976242</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>2.75835886976242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -632,10 +632,10 @@
         <v>43101.625</v>
       </c>
       <c r="B17" t="n">
-        <v>3.186692330624577</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>3.186692330624577</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +643,10 @@
         <v>43101.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>3.156782558528777</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>3.156782558528777</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -654,10 +654,10 @@
         <v>43101.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>2.285879118907595</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>2.285879118907595</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -665,10 +665,10 @@
         <v>43101.75</v>
       </c>
       <c r="B20" t="n">
-        <v>4.117210566439198</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>4.117210566439198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -676,10 +676,10 @@
         <v>43101.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>10.27487108205195</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>10.27487108205195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -687,10 +687,10 @@
         <v>43101.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>13.87122552781372</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>13.87122552781372</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -698,10 +698,10 @@
         <v>43101.875</v>
       </c>
       <c r="B23" t="n">
-        <v>7.091968568126363</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>7.091968568126363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -709,10 +709,10 @@
         <v>43101.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>3.801038602806567</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>3.801038602806567</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -720,10 +720,10 @@
         <v>43101.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>3.289634830491467</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>3.289634830491467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -731,10 +731,10 @@
         <v>43102</v>
       </c>
       <c r="B26" t="n">
-        <v>1.723045843221649</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.723045843221649</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12.25421529412514</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>144.1324583736267</v>
+        <v>2106.75</v>
       </c>
     </row>
     <row r="6">
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2757.066666666667</v>
       </c>
     </row>
     <row r="7">
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.970458967280538</v>
+        <v>22.37625</v>
       </c>
     </row>
   </sheetData>
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>597.3773689855281</v>
+        <v>4500</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.26218998744227</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -955,13 +955,13 @@
         <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>0.554028571</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.554028571</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -972,13 +972,13 @@
         <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.469628571</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.469628571</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -989,13 +989,13 @@
         <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>7.245377247649912</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>7.245377247649912</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1006,13 +1006,13 @@
         <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.549585714</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.549585714</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1023,13 +1023,13 @@
         <v>43101.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.6267</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>0.6267</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1040,13 +1040,13 @@
         <v>43101.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>3.771141997591101</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3.771141997591101</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1057,13 +1057,13 @@
         <v>43101.25</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>6.202756082034924</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>6.202756082034924</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1074,13 +1074,13 @@
         <v>43101.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>5.529049211325205</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>5.529049211325205</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1091,13 +1091,13 @@
         <v>43101.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>5.907222702238744</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>5.907222702238744</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1108,16 +1108,16 @@
         <v>43101.375</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>3.144218023214221</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0.004434173400726668</v>
+        <v>4.252761373395888</v>
       </c>
       <c r="E11" t="n">
-        <v>0.004434173400726668</v>
+        <v>1.108543350181667</v>
       </c>
     </row>
     <row r="12">
@@ -1128,13 +1128,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>5.586883168290823</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0330909158605925</v>
+        <v>2.6858457968573</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0330909158605925</v>
+        <v>8.272728965148124</v>
       </c>
     </row>
     <row r="13">
@@ -1145,13 +1145,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>46.5148636963539</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2035856265144559</v>
+        <v>4.381542932260076</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2035856265144559</v>
+        <v>50.89640662861397</v>
       </c>
     </row>
     <row r="14">
@@ -1162,13 +1162,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>4.562246680843671</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07179657458966061</v>
+        <v>13.38689696657148</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07179657458966061</v>
+        <v>17.94914364741515</v>
       </c>
     </row>
     <row r="15">
@@ -1179,13 +1179,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>6.47183429359802</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03016705145839208</v>
+        <v>1.069928571</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03016705145839208</v>
+        <v>7.54176286459802</v>
       </c>
     </row>
     <row r="16">
@@ -1193,13 +1193,13 @@
         <v>43101.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>2.825040474208677</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>2.825040474208677</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1210,13 +1210,13 @@
         <v>43101.625</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>3.212498410367769</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>3.212498410367769</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1227,13 +1227,13 @@
         <v>43101.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.398457143</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1.398457143</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1244,13 +1244,13 @@
         <v>43101.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1.839342857</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1.839342857</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1261,13 +1261,13 @@
         <v>43101.75</v>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>2.005842857</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2.005842857</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1278,13 +1278,13 @@
         <v>43101.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>8.649585714000001</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>8.649585714000001</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1295,13 +1295,13 @@
         <v>43101.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>12.11352857</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>12.11352857</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -1312,13 +1312,13 @@
         <v>43101.875</v>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>25.47546728336945</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>15.02745821417941</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>10.44800906919004</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1329,13 +1329,13 @@
         <v>43101.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>1.689628571</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>1.689628571</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
@@ -1346,13 +1346,13 @@
         <v>43101.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>0.813671429</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.813671429</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1363,13 +1363,13 @@
         <v>43102</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>0.577228571</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.577228571</v>
       </c>
       <c r="E26" t="n">
         <v>0</v>
@@ -1545,10 +1545,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.004434173400726668</v>
+        <v>1.108543350181667</v>
       </c>
       <c r="D11" t="n">
-        <v>0.004434173400726668</v>
+        <v>1.108543350181667</v>
       </c>
     </row>
     <row r="12">
@@ -1559,10 +1559,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0330909158605925</v>
+        <v>8.272728965148124</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0330909158605925</v>
+        <v>8.272728965148124</v>
       </c>
     </row>
     <row r="13">
@@ -1573,10 +1573,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2035856265144559</v>
+        <v>50.89640662861397</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2035856265144559</v>
+        <v>50.89640662861397</v>
       </c>
     </row>
     <row r="14">
@@ -1587,10 +1587,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07179657458966061</v>
+        <v>17.94914364741515</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07179657458966061</v>
+        <v>17.94914364741515</v>
       </c>
     </row>
     <row r="15">
@@ -1601,10 +1601,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03016705145839208</v>
+        <v>7.54176286459802</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03016705145839208</v>
+        <v>7.54176286459802</v>
       </c>
     </row>
     <row r="16">
@@ -1807,16 +1807,16 @@
         <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>2.932054282126365</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>0.554028571</v>
       </c>
       <c r="D2" t="n">
-        <v>3.486082853126365</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.554028571</v>
       </c>
     </row>
     <row r="3">
@@ -1824,16 +1824,16 @@
         <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>2.932054282126364</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0.469628571</v>
       </c>
       <c r="D3" t="n">
-        <v>3.401682853126363</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.469628571</v>
       </c>
     </row>
     <row r="4">
@@ -1841,16 +1841,16 @@
         <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>2.932054282126365</v>
+        <v>6.788420104649911</v>
       </c>
       <c r="C4" t="n">
         <v>0.456957143</v>
       </c>
       <c r="D4" t="n">
-        <v>3.389011425126365</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>7.245377247649912</v>
       </c>
     </row>
     <row r="5">
@@ -1858,16 +1858,16 @@
         <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>2.932054282126364</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
         <v>0.549585714</v>
       </c>
       <c r="D5" t="n">
-        <v>3.481639996126364</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.549585714</v>
       </c>
     </row>
     <row r="6">
@@ -1875,16 +1875,16 @@
         <v>43101.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>2.932054282126364</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0.6267</v>
       </c>
       <c r="D6" t="n">
-        <v>3.558754282126364</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>0.6267</v>
       </c>
     </row>
     <row r="7">
@@ -1892,16 +1892,16 @@
         <v>43101.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>2.932054282126364</v>
+        <v>3.160941997591101</v>
       </c>
       <c r="C7" t="n">
         <v>0.6102</v>
       </c>
       <c r="D7" t="n">
-        <v>3.542254282126363</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3.771141997591101</v>
       </c>
     </row>
     <row r="8">
@@ -1909,16 +1909,16 @@
         <v>43101.25</v>
       </c>
       <c r="B8" t="n">
-        <v>2.932054282126364</v>
+        <v>2.948527511034924</v>
       </c>
       <c r="C8" t="n">
         <v>3.254228571</v>
       </c>
       <c r="D8" t="n">
-        <v>6.186282853126365</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>6.202756082034924</v>
       </c>
     </row>
     <row r="9">
@@ -1926,16 +1926,16 @@
         <v>43101.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>2.776135053191083</v>
+        <v>2.792563497325205</v>
       </c>
       <c r="C9" t="n">
         <v>2.736485714</v>
       </c>
       <c r="D9" t="n">
-        <v>5.512620767191083</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>5.529049211325205</v>
       </c>
     </row>
     <row r="10">
@@ -1943,16 +1943,16 @@
         <v>43101.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>2.435240473042553</v>
+        <v>2.451579845238745</v>
       </c>
       <c r="C10" t="n">
         <v>3.455642857</v>
       </c>
       <c r="D10" t="n">
-        <v>5.890883330042554</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>5.907222702238744</v>
       </c>
     </row>
     <row r="11">
@@ -1960,16 +1960,16 @@
         <v>43101.375</v>
       </c>
       <c r="B11" t="n">
-        <v>1.672326751202708</v>
+        <v>1.688489944395888</v>
       </c>
       <c r="C11" t="n">
         <v>2.564271429</v>
       </c>
       <c r="D11" t="n">
-        <v>4.232164006801982</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.004434173400726668</v>
+        <v>4.252761373395888</v>
       </c>
     </row>
     <row r="12">
@@ -1977,16 +1977,16 @@
         <v>43101.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>1.379140530315636</v>
+        <v>1.3952600828573</v>
       </c>
       <c r="C12" t="n">
         <v>1.290585714</v>
       </c>
       <c r="D12" t="n">
-        <v>2.636635328455043</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0330909158605925</v>
+        <v>2.6858457968573</v>
       </c>
     </row>
     <row r="13">
@@ -1994,16 +1994,16 @@
         <v>43101.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>0.06708938166208164</v>
+        <v>0.08261436126007536</v>
       </c>
       <c r="C13" t="n">
         <v>4.298928571</v>
       </c>
       <c r="D13" t="n">
-        <v>4.162432326147626</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2035856265144559</v>
+        <v>4.381542932260076</v>
       </c>
     </row>
     <row r="14">
@@ -2011,16 +2011,16 @@
         <v>43101.5</v>
       </c>
       <c r="B14" t="n">
-        <v>1.520133461352607</v>
+        <v>11.45105410957148</v>
       </c>
       <c r="C14" t="n">
         <v>1.935842857</v>
       </c>
       <c r="D14" t="n">
-        <v>3.384179743762946</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.07179657458966061</v>
+        <v>13.38689696657148</v>
       </c>
     </row>
     <row r="15">
@@ -2034,10 +2034,10 @@
         <v>1.069928571</v>
       </c>
       <c r="D15" t="n">
-        <v>1.039761519541608</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03016705145839208</v>
+        <v>1.069928571</v>
       </c>
     </row>
     <row r="16">
@@ -2045,16 +2045,16 @@
         <v>43101.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>1.69967315576242</v>
+        <v>1.766354760208677</v>
       </c>
       <c r="C16" t="n">
         <v>1.058685714</v>
       </c>
       <c r="D16" t="n">
-        <v>2.75835886976242</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>2.825040474208677</v>
       </c>
     </row>
     <row r="17">
@@ -2062,16 +2062,16 @@
         <v>43101.625</v>
       </c>
       <c r="B17" t="n">
-        <v>1.466935187624577</v>
+        <v>1.492741267367769</v>
       </c>
       <c r="C17" t="n">
         <v>1.719757143</v>
       </c>
       <c r="D17" t="n">
-        <v>3.186692330624577</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>3.212498410367769</v>
       </c>
     </row>
     <row r="18">
@@ -2079,16 +2079,16 @@
         <v>43101.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>1.758325415528777</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>1.398457143</v>
       </c>
       <c r="D18" t="n">
-        <v>3.156782558528777</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>1.398457143</v>
       </c>
     </row>
     <row r="19">
@@ -2096,16 +2096,16 @@
         <v>43101.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4465362619075952</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>1.839342857</v>
       </c>
       <c r="D19" t="n">
-        <v>2.285879118907595</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1.839342857</v>
       </c>
     </row>
     <row r="20">
@@ -2113,16 +2113,16 @@
         <v>43101.75</v>
       </c>
       <c r="B20" t="n">
-        <v>2.111367709439198</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>2.005842857</v>
       </c>
       <c r="D20" t="n">
-        <v>4.117210566439198</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>2.005842857</v>
       </c>
     </row>
     <row r="21">
@@ -2130,16 +2130,16 @@
         <v>43101.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>1.625285368051953</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>8.649585714000001</v>
       </c>
       <c r="D21" t="n">
-        <v>10.27487108205195</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>8.649585714000001</v>
       </c>
     </row>
     <row r="22">
@@ -2147,16 +2147,16 @@
         <v>43101.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>1.757696957813716</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>12.11352857</v>
       </c>
       <c r="D22" t="n">
-        <v>13.87122552781372</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>12.11352857</v>
       </c>
     </row>
     <row r="23">
@@ -2164,16 +2164,16 @@
         <v>43101.875</v>
       </c>
       <c r="B23" t="n">
-        <v>2.932054282126364</v>
+        <v>6.288094783190043</v>
       </c>
       <c r="C23" t="n">
         <v>4.159914286</v>
       </c>
       <c r="D23" t="n">
-        <v>7.091968568126363</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>10.44800906919004</v>
       </c>
     </row>
     <row r="24">
@@ -2181,16 +2181,16 @@
         <v>43101.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>2.111410031806567</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>1.689628571</v>
       </c>
       <c r="D24" t="n">
-        <v>3.801038602806567</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>1.689628571</v>
       </c>
     </row>
     <row r="25">
@@ -2198,16 +2198,16 @@
         <v>43101.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>2.475963401491467</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0.813671429</v>
       </c>
       <c r="D25" t="n">
-        <v>3.289634830491467</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.813671429</v>
       </c>
     </row>
     <row r="26">
@@ -2215,16 +2215,16 @@
         <v>43102</v>
       </c>
       <c r="B26" t="n">
-        <v>1.145817272221649</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0.577228571</v>
       </c>
       <c r="D26" t="n">
-        <v>1.723045843221649</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>0.577228571</v>
       </c>
     </row>
   </sheetData>
@@ -2273,16 +2273,16 @@
         <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>12.35916285015212</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12.35916285015212</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>4.199975437480393</v>
+        <v>24.41023943949497</v>
       </c>
     </row>
     <row r="3">
@@ -2290,16 +2290,16 @@
         <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.411638906367753</v>
+        <v>11.13843355808191</v>
       </c>
     </row>
     <row r="4">
@@ -2307,16 +2307,16 @@
         <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>12.42673989188693</v>
+        <v>28.77093082197741</v>
       </c>
       <c r="C4" t="n">
-        <v>12.42673989188693</v>
+        <v>13.17307588</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>15.59785494197741</v>
       </c>
       <c r="E4" t="n">
-        <v>2.651107476087512</v>
+        <v>26.64435025980561</v>
       </c>
     </row>
     <row r="5">
@@ -2324,16 +2324,16 @@
         <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1.858796335326218</v>
+        <v>13.36468957599664</v>
       </c>
     </row>
     <row r="6">
@@ -2341,16 +2341,16 @@
         <v>43101.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>12.32546143541226</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>12.32546143541226</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.901187205670741</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2358,13 +2358,13 @@
         <v>43101.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>12.42673989188692</v>
+        <v>13.39682019424264</v>
       </c>
       <c r="C7" t="n">
-        <v>12.42673989188692</v>
+        <v>13.31630662</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -2375,13 +2375,13 @@
         <v>43101.25</v>
       </c>
       <c r="B8" t="n">
-        <v>12.42673989188692</v>
+        <v>12.49655733424264</v>
       </c>
       <c r="C8" t="n">
         <v>12.41604376</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -2392,13 +2392,13 @@
         <v>43101.29166666666</v>
       </c>
       <c r="B9" t="n">
-        <v>11.79799179188692</v>
+        <v>11.86780923424264</v>
       </c>
       <c r="C9" t="n">
         <v>11.78729566</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -2409,13 +2409,13 @@
         <v>43101.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>10.40567895188692</v>
+        <v>10.47549639424264</v>
       </c>
       <c r="C10" t="n">
         <v>10.39498282</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -2426,13 +2426,13 @@
         <v>43101.375</v>
       </c>
       <c r="B11" t="n">
-        <v>7.223670171886922</v>
+        <v>7.293487614242636</v>
       </c>
       <c r="C11" t="n">
         <v>7.21297404</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -2443,13 +2443,13 @@
         <v>43101.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>5.973370800886922</v>
+        <v>6.043188243242636</v>
       </c>
       <c r="C12" t="n">
         <v>5.962674669</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -2460,13 +2460,13 @@
         <v>43101.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3017079028869217</v>
+        <v>0.3715253452426365</v>
       </c>
       <c r="C13" t="n">
         <v>0.291011771</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01069613188692177</v>
+        <v>0.0805135742426365</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -2477,16 +2477,16 @@
         <v>43101.5</v>
       </c>
       <c r="B14" t="n">
-        <v>6.946171296037279</v>
+        <v>52.325</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6.946171296037279</v>
+        <v>52.325</v>
       </c>
       <c r="E14" t="n">
-        <v>6.935475164150357</v>
+        <v>52.24448642575736</v>
       </c>
     </row>
     <row r="15">
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>3.90959104713434</v>
+        <v>49.10231151640725</v>
       </c>
     </row>
     <row r="16">
@@ -2511,16 +2511,16 @@
         <v>43101.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>7.704925176450304</v>
+        <v>8.007204924272527</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7587538804130256</v>
+        <v>4.653638737</v>
       </c>
       <c r="D16" t="n">
-        <v>6.946171296037279</v>
+        <v>3.353566187272527</v>
       </c>
       <c r="E16" t="n">
-        <v>6.946171296037279</v>
+        <v>52.325</v>
       </c>
     </row>
     <row r="17">
@@ -2528,16 +2528,16 @@
         <v>43101.625</v>
       </c>
       <c r="B17" t="n">
-        <v>6.614569378014208</v>
+        <v>6.730931781940396</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>6.596748574</v>
       </c>
       <c r="D17" t="n">
-        <v>6.614569378014208</v>
+        <v>0.1341832079403957</v>
       </c>
       <c r="E17" t="n">
-        <v>6.946171296037279</v>
+        <v>52.325</v>
       </c>
     </row>
     <row r="18">
@@ -2545,16 +2545,16 @@
         <v>43101.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>7.865267041014208</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9190957449769295</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6.946171296037279</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>6.946171296037279</v>
+        <v>44.3433705550596</v>
       </c>
     </row>
     <row r="19">
@@ -2562,16 +2562,16 @@
         <v>43101.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>1.976153827976928</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.95833302396272</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0178208040142076</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>35.31286976631884</v>
       </c>
     </row>
     <row r="20">
@@ -2579,16 +2579,16 @@
         <v>43101.75</v>
       </c>
       <c r="B20" t="n">
-        <v>9.368974598886922</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>9.358278467</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01069613188692177</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>25.83785739473363</v>
       </c>
     </row>
     <row r="21">
@@ -2596,16 +2596,16 @@
         <v>43101.79166666666</v>
       </c>
       <c r="B21" t="n">
-        <v>7.250749606886922</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>7.240053475</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01069613188692177</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>18.49078851382524</v>
       </c>
     </row>
     <row r="22">
@@ -2613,16 +2613,16 @@
         <v>43101.83333333334</v>
       </c>
       <c r="B22" t="n">
-        <v>7.841466351948823</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>6.579958661</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>1.261507690948823</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1.250811559061901</v>
+        <v>11.81135031878672</v>
       </c>
     </row>
     <row r="23">
@@ -2630,16 +2630,16 @@
         <v>43101.875</v>
       </c>
       <c r="B23" t="n">
-        <v>13.0805284114385</v>
+        <v>28.0525510618056</v>
       </c>
       <c r="C23" t="n">
         <v>7.373189588</v>
       </c>
       <c r="D23" t="n">
-        <v>5.707338823438502</v>
+        <v>20.6793614738056</v>
       </c>
       <c r="E23" t="n">
-        <v>6.946171296037279</v>
+        <v>32.39808334314499</v>
       </c>
     </row>
     <row r="24">
@@ -2647,16 +2647,16 @@
         <v>43101.91666666666</v>
       </c>
       <c r="B24" t="n">
-        <v>9.344081036014206</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>9.326260231999999</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0178208040142076</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>6.946171296037279</v>
+        <v>22.9580788963761</v>
       </c>
     </row>
     <row r="25">
@@ -2664,16 +2664,16 @@
         <v>43101.95833333334</v>
       </c>
       <c r="B25" t="n">
-        <v>10.92805762401421</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>10.91023682</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0178208040142076</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>6.946171296037279</v>
+        <v>11.94378045273504</v>
       </c>
     </row>
     <row r="26">
@@ -2681,10 +2681,10 @@
         <v>43102</v>
       </c>
       <c r="B26" t="n">
-        <v>4.922665677976928</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>4.922665677976928</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -2960,10 +2960,10 @@
         <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>12.35916285015212</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7854419998478797</v>
+        <v>13.14460485</v>
       </c>
       <c r="D2" t="n">
         <v>13.14460485</v>
@@ -2974,10 +2974,10 @@
         <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7733324939554027</v>
+        <v>13.16625478</v>
       </c>
       <c r="D3" t="n">
         <v>13.16625478</v>
@@ -2988,10 +2988,10 @@
         <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>12.42673989188693</v>
+        <v>13.17307588</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7463359881130742</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>13.17307588</v>
@@ -3002,10 +3002,10 @@
         <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>12.3929222860446</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7788957739554032</v>
+        <v>13.17181806</v>
       </c>
       <c r="D5" t="n">
         <v>13.17181806</v>
@@ -3016,10 +3016,10 @@
         <v>43101.16666666666</v>
       </c>
       <c r="B6" t="n">
-        <v>12.32546143541226</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9450064345877411</v>
+        <v>13.27046787</v>
       </c>
       <c r="D6" t="n">
         <v>13.27046787</v>
@@ -3030,10 +3030,10 @@
         <v>43101.20833333334</v>
       </c>
       <c r="B7" t="n">
-        <v>12.42673989188692</v>
+        <v>13.31630662</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8895667281130795</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>13.31630662</v>
@@ -3156,10 +3156,10 @@
         <v>43101.58333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7587538804130256</v>
+        <v>4.653638737</v>
       </c>
       <c r="C16" t="n">
-        <v>3.894884856586974</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>4.653638737</v>
@@ -3170,10 +3170,10 @@
         <v>43101.625</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>6.596748574</v>
       </c>
       <c r="C17" t="n">
-        <v>6.596748574</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>6.596748574</v>
@@ -3184,10 +3184,10 @@
         <v>43101.66666666666</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9190957449769295</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>6.92835049202307</v>
+        <v>7.847446237</v>
       </c>
       <c r="D18" t="n">
         <v>7.847446237</v>
@@ -3198,10 +3198,10 @@
         <v>43101.70833333334</v>
       </c>
       <c r="B19" t="n">
-        <v>1.95833302396272</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>6.946171296037279</v>
+        <v>8.904504319999999</v>
       </c>
       <c r="D19" t="n">
         <v>8.904504319999999</v>
@@ -3212,10 +3212,10 @@
         <v>43101.75</v>
       </c>
       <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
         <v>9.358278467</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>9.358278467</v>
@@ -3226,10 +3226,10 @@
         <v>43101.79166666666</v>
       </c>
       <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
         <v>7.240053475</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>7.240053475</v>
@@ -3240,10 +3240,10 @@
         <v>43101.83333333334</v>
       </c>
       <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
         <v>6.579958661</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>6.579958661</v>
@@ -3268,10 +3268,10 @@
         <v>43101.91666666666</v>
       </c>
       <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
         <v>9.326260231999999</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>9.326260231999999</v>
@@ -3282,10 +3282,10 @@
         <v>43101.95833333334</v>
       </c>
       <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
         <v>10.91023682</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>10.91023682</v>
@@ -3296,10 +3296,10 @@
         <v>43102</v>
       </c>
       <c r="B26" t="n">
-        <v>4.922665677976928</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>6.928350492023071</v>
+        <v>11.85101617</v>
       </c>
       <c r="D26" t="n">
         <v>11.85101617</v>
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22.33006306698274</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -3662,7 +3662,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3762.647343642219</v>
+        <v>58998.22712595509</v>
       </c>
     </row>
     <row r="5">
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0</v>
+        <v>-7.034695744793924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed test_mpc_example for new storage content sheet and labels
</commit_message>
<xml_diff>
--- a/tests/test_examples/expected_files/results_MPC_example_2018_01_01__00_00_00.xlsx
+++ b/tests/test_examples/expected_files/results_MPC_example_2018_01_01__00_00_00.xlsx
@@ -15,10 +15,11 @@
     <sheet name="dhwSourceBus__Building1" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="spaceHeatingBus__Building1" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="shDemandBus__Building1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="costs__Building1" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="env_impacts__Building1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="capStorages__Building1" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="capTransformers__Building1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="storage_content__Building1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="costs__Building1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="env_impacts__Building1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="capStorages__Building1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="capTransformers__Building1" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -748,6 +749,70 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>electricityResource__Building1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>naturalGasResource__Building1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Investment</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>58998.22712595509</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Feed-in</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-7.034695744793923</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -804,21 +869,21 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>electricalStorage__Building1</t>
+          <t>shStorage__Building1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2757.066666666667</v>
+        <v>22.37625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>shStorage__Building1</t>
+          <t>electricalStorage__Building1</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22.37625</v>
+        <v>2757.066666666667</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -848,21 +913,21 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>electricalStorage__Building1</t>
+          <t>shStorage__Building1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>200</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>shStorage__Building1</t>
+          <t>electricalStorage__Building1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4500</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1142,10 +1207,10 @@
         <v>43101.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>15.0274582141794</v>
       </c>
       <c r="C13" t="n">
-        <v>46.5148636963539</v>
+        <v>61.5423219105333</v>
       </c>
       <c r="D13" t="n">
         <v>4.381542932260076</v>
@@ -1312,10 +1377,10 @@
         <v>43101.875</v>
       </c>
       <c r="B23" t="n">
-        <v>25.47546728336945</v>
+        <v>10.44800906919004</v>
       </c>
       <c r="C23" t="n">
-        <v>15.02745821417941</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>10.44800906919004</v>
@@ -2238,7 +2303,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2262,11 +2327,6 @@
           <t>(('shSourceBus__Building1', 'shStorage__Building1'), 'flow')</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>storage_content</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -2281,9 +2341,6 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
-        <v>24.41023943949497</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -2298,9 +2355,6 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="n">
-        <v>11.13843355808191</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -2315,9 +2369,6 @@
       <c r="D4" t="n">
         <v>15.59785494197741</v>
       </c>
-      <c r="E4" t="n">
-        <v>26.64435025980561</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -2332,9 +2383,6 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
-      <c r="E5" t="n">
-        <v>13.36468957599664</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -2349,9 +2397,6 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -2366,9 +2411,6 @@
       <c r="D7" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -2383,9 +2425,6 @@
       <c r="D8" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -2400,9 +2439,6 @@
       <c r="D9" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -2417,9 +2453,6 @@
       <c r="D10" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -2434,9 +2467,6 @@
       <c r="D11" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -2451,9 +2481,6 @@
       <c r="D12" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -2468,9 +2495,6 @@
       <c r="D13" t="n">
         <v>0.0805135742426365</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -2485,9 +2509,6 @@
       <c r="D14" t="n">
         <v>52.325</v>
       </c>
-      <c r="E14" t="n">
-        <v>52.24448642575736</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -2502,9 +2523,6 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
-      <c r="E15" t="n">
-        <v>49.10231151640725</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -2519,9 +2537,6 @@
       <c r="D16" t="n">
         <v>3.353566187272527</v>
       </c>
-      <c r="E16" t="n">
-        <v>52.325</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -2536,9 +2551,6 @@
       <c r="D17" t="n">
         <v>0.1341832079403957</v>
       </c>
-      <c r="E17" t="n">
-        <v>52.325</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -2553,9 +2565,6 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E18" t="n">
-        <v>44.3433705550596</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -2570,9 +2579,6 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
-      <c r="E19" t="n">
-        <v>35.31286976631884</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -2587,9 +2593,6 @@
       <c r="D20" t="n">
         <v>0</v>
       </c>
-      <c r="E20" t="n">
-        <v>25.83785739473363</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -2604,9 +2607,6 @@
       <c r="D21" t="n">
         <v>0</v>
       </c>
-      <c r="E21" t="n">
-        <v>18.49078851382524</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -2621,9 +2621,6 @@
       <c r="D22" t="n">
         <v>0</v>
       </c>
-      <c r="E22" t="n">
-        <v>11.81135031878672</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -2638,9 +2635,6 @@
       <c r="D23" t="n">
         <v>20.6793614738056</v>
       </c>
-      <c r="E23" t="n">
-        <v>32.39808334314499</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -2655,9 +2649,6 @@
       <c r="D24" t="n">
         <v>0</v>
       </c>
-      <c r="E24" t="n">
-        <v>22.9580788963761</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -2672,9 +2663,6 @@
       <c r="D25" t="n">
         <v>0</v>
       </c>
-      <c r="E25" t="n">
-        <v>11.94378045273504</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -2687,9 +2675,6 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3622,7 +3607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3631,48 +3616,290 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>shStorage__B001_storage_content</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>electricalStorage__B001_storage_content</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>electricityResource__Building1</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>43101</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>24.41023943949497</v>
+      </c>
+      <c r="C2" t="n">
+        <v>109.3557807313954</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>naturalGasResource__Building1</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>43101.04166666666</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>11.13843355808191</v>
+      </c>
+      <c r="C3" t="n">
+        <v>108.8097009976744</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Investment</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>43101.08333333334</v>
       </c>
       <c r="B4" t="n">
-        <v>58998.22712595509</v>
+        <v>26.64435025980561</v>
+      </c>
+      <c r="C4" t="n">
+        <v>100.3848437329652</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Feed-in</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>43101.125</v>
       </c>
       <c r="B5" t="n">
-        <v>-7.034695744793924</v>
+        <v>13.36468957599664</v>
+      </c>
+      <c r="C5" t="n">
+        <v>99.74579057715127</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>43101.16666666666</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>99.01706964691871</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>43101.20833333334</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>94.63202081251046</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>43101.25</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>87.41951374037683</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>43101.29166666666</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>80.9903867504638</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>43101.33333333334</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>74.12152314320944</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>43101.375</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>70.4654556743557</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>43101.41666666666</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>70.4654556743557</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>43101.45833333334</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>52.99166705321686</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>43101.5</v>
+      </c>
+      <c r="B14" t="n">
+        <v>52.24448642575736</v>
+      </c>
+      <c r="C14" t="n">
+        <v>52.99166705321686</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>43101.54166666666</v>
+      </c>
+      <c r="B15" t="n">
+        <v>49.10231151640725</v>
+      </c>
+      <c r="C15" t="n">
+        <v>52.99166705321686</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>43101.58333333334</v>
+      </c>
+      <c r="B16" t="n">
+        <v>52.325</v>
+      </c>
+      <c r="C16" t="n">
+        <v>49.70673626925328</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>43101.625</v>
+      </c>
+      <c r="B17" t="n">
+        <v>52.325</v>
+      </c>
+      <c r="C17" t="n">
+        <v>45.97127300138378</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>43101.66666666666</v>
+      </c>
+      <c r="B18" t="n">
+        <v>44.3433705550596</v>
+      </c>
+      <c r="C18" t="n">
+        <v>44.34516004440703</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>43101.70833333334</v>
+      </c>
+      <c r="B19" t="n">
+        <v>35.31286976631884</v>
+      </c>
+      <c r="C19" t="n">
+        <v>42.20638928045354</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>43101.75</v>
+      </c>
+      <c r="B20" t="n">
+        <v>25.83785739473363</v>
+      </c>
+      <c r="C20" t="n">
+        <v>39.87401386533726</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>43101.79166666666</v>
+      </c>
+      <c r="B21" t="n">
+        <v>18.49078851382524</v>
+      </c>
+      <c r="C21" t="n">
+        <v>29.81635605836052</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>43101.83333333334</v>
+      </c>
+      <c r="B22" t="n">
+        <v>11.81135031878672</v>
+      </c>
+      <c r="C22" t="n">
+        <v>15.73085772115121</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>43101.875</v>
+      </c>
+      <c r="B23" t="n">
+        <v>32.39808334314499</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3.58200996627907</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>43101.91666666666</v>
+      </c>
+      <c r="B24" t="n">
+        <v>22.9580788963761</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.617325581395349</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>43101.95833333334</v>
+      </c>
+      <c r="B25" t="n">
+        <v>11.94378045273504</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.6711960127906977</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>43102</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>